<commit_message>
add aquaculture column to ladder parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-salmon ladder collection.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-salmon ladder collection.xlsx
@@ -29,23 +29,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. 1999</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. 1999</t>
         </r>
       </text>
     </comment>
@@ -53,23 +42,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. Jan</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. Jan</t>
         </r>
       </text>
     </comment>
@@ -77,23 +55,25 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. 1</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Must match a site name in the database</t>
         </r>
       </text>
     </comment>
@@ -101,23 +81,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-True/False value.  Eg. 1/0, y/n</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>True/False value.  Eg. 1/0, y/n</t>
         </r>
       </text>
     </comment>
@@ -125,23 +94,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. Bonell</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. Bonell</t>
         </r>
       </text>
     </comment>
@@ -149,23 +107,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-eg. FP</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. 2021 FP</t>
         </r>
       </text>
     </comment>
@@ -173,23 +120,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional, units can be (cm) or (mm)</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional, units can be (cm) or (mm)</t>
         </r>
       </text>
     </comment>
@@ -197,23 +133,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional, M/F/IT/I</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional, M/F/IT/I</t>
         </r>
       </text>
     </comment>
@@ -221,23 +146,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -245,23 +159,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -269,23 +172,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional, True/False value, eg. 1/0, Y/N</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional, True/False value, eg. 1/0, Y/N</t>
         </r>
       </text>
     </comment>
@@ -293,23 +185,12 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Eg. AB, CD</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill if individual is associated with an aquaculture site.  Value must match name of an aquaculture site code in the database</t>
         </r>
       </text>
     </comment>
@@ -317,23 +198,25 @@
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Stoyel, Quentin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Optional</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. AB, CD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -342,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Site</t>
   </si>
@@ -390,6 +273,9 @@
   </si>
   <si>
     <t>Wild Return</t>
+  </si>
+  <si>
+    <t>Aquaculture Site</t>
   </si>
 </sst>
 </file>
@@ -533,7 +419,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -543,7 +428,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1253,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P3"/>
+  <dimension ref="A3:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,10 +1154,11 @@
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1316,9 +1202,12 @@
         <v>12</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>